<commit_message>
LE4 | Adjusted LE4-7 with new changes from sir james
</commit_message>
<xml_diff>
--- a/LE_04/_MATERIAL_/WorkBook2_Attempt2.xlsx
+++ b/LE_04/_MATERIAL_/WorkBook2_Attempt2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\notjo\OneDrive\Desktop\USC\USC-Year3-Sem2\3201-EmbeddedSystems\Labs\LE_04\_MATERIAL_\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CFACF74-DF11-4DE4-A4C0-9236D9671387}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{315B7B91-6D10-46D9-A127-30E1E68F4A7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22046" yWindow="-103" windowWidth="22149" windowHeight="13200" xr2:uid="{D68BE116-9CE4-4393-B23E-E2B8785469CA}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="13185" windowHeight="15585" xr2:uid="{D68BE116-9CE4-4393-B23E-E2B8785469CA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -600,8 +600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{443F6C2F-298E-47EE-9F3A-65C49EA70655}">
   <dimension ref="A1:L34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -721,7 +721,7 @@
         <v>16</v>
       </c>
       <c r="G3" s="7">
-        <f t="shared" ref="G3:G16" si="3">ROUNDDOWN(D3/(E3*F3),0)</f>
+        <f t="shared" ref="G3:G15" si="3">ROUNDDOWN(D3/(E3*F3),0)</f>
         <v>52</v>
       </c>
       <c r="H3" s="9" t="str">

</xml_diff>

<commit_message>
LE5 | ADC Reading to LED BAR and Seven Seg
</commit_message>
<xml_diff>
--- a/LE_04/_MATERIAL_/WorkBook2_Attempt2.xlsx
+++ b/LE_04/_MATERIAL_/WorkBook2_Attempt2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\notjo\OneDrive\Desktop\USC\USC-Year3-Sem2\3201-EmbeddedSystems\Labs\LE_04\_MATERIAL_\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{315B7B91-6D10-46D9-A127-30E1E68F4A7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B9AC4D2-B343-4FC3-818E-2E20FA5B5122}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="13185" windowHeight="15585" xr2:uid="{D68BE116-9CE4-4393-B23E-E2B8785469CA}"/>
+    <workbookView xWindow="-86" yWindow="0" windowWidth="11143" windowHeight="13080" xr2:uid="{D68BE116-9CE4-4393-B23E-E2B8785469CA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="32">
   <si>
     <t>FREQUENCIES</t>
   </si>
@@ -598,10 +598,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{443F6C2F-298E-47EE-9F3A-65C49EA70655}">
-  <dimension ref="A1:L34"/>
+  <dimension ref="A1:L51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" topLeftCell="F10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1374,8 +1374,14 @@
         <f>(B20*E20)</f>
         <v>3.3333333333333338E-4</v>
       </c>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
+      <c r="I20" s="3">
+        <f>HEX2DEC(G20)</f>
+        <v>83</v>
+      </c>
+      <c r="J20" s="5">
+        <f t="shared" ref="J20:J28" si="6">(B20*E20)/((1/C20)*16)</f>
+        <v>83.333333333333343</v>
+      </c>
       <c r="K20" s="4"/>
       <c r="L20" s="4"/>
     </row>
@@ -1393,23 +1399,29 @@
         <v>16</v>
       </c>
       <c r="E21" s="3">
-        <f t="shared" ref="E21:E24" si="6">1/A21</f>
+        <f t="shared" ref="E21:E24" si="7">1/A21</f>
         <v>3.3333333333333335E-3</v>
       </c>
       <c r="F21" s="11" t="str">
-        <f t="shared" ref="F21:F34" si="7">DEC2HEX(ROUND((E21/(4*(2.5*10^-7)*D21))-1,0))</f>
+        <f t="shared" ref="F21:F34" si="8">DEC2HEX(ROUND((E21/(4*(2.5*10^-7)*D21))-1,0))</f>
         <v>CF</v>
       </c>
       <c r="G21" s="14" t="str">
-        <f t="shared" ref="G21:G34" si="8">DEC2HEX(ROUND((B21*E21)/((1/C21)*16),0))</f>
+        <f t="shared" ref="G21:G34" si="9">DEC2HEX(ROUND((B21*E21)/((1/C21)*16),0))</f>
         <v>D0</v>
       </c>
       <c r="H21" s="18">
-        <f t="shared" ref="H21:H34" si="9">(B21*E21)</f>
+        <f t="shared" ref="H21:H34" si="10">(B21*E21)</f>
         <v>8.3333333333333339E-4</v>
       </c>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
+      <c r="I21" s="3">
+        <f t="shared" ref="I21:I34" si="11">HEX2DEC(G21)</f>
+        <v>208</v>
+      </c>
+      <c r="J21" s="5">
+        <f t="shared" si="6"/>
+        <v>208.33333333333334</v>
+      </c>
       <c r="K21" s="4"/>
       <c r="L21" s="4"/>
     </row>
@@ -1427,23 +1439,29 @@
         <v>16</v>
       </c>
       <c r="E22" s="3">
+        <f t="shared" si="7"/>
+        <v>3.3333333333333335E-3</v>
+      </c>
+      <c r="F22" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>CF</v>
+      </c>
+      <c r="G22" s="14" t="str">
+        <f t="shared" si="9"/>
+        <v>1A1</v>
+      </c>
+      <c r="H22" s="18">
+        <f t="shared" si="10"/>
+        <v>1.6666666666666668E-3</v>
+      </c>
+      <c r="I22" s="3">
+        <f t="shared" si="11"/>
+        <v>417</v>
+      </c>
+      <c r="J22" s="5">
         <f t="shared" si="6"/>
-        <v>3.3333333333333335E-3</v>
-      </c>
-      <c r="F22" s="11" t="str">
-        <f t="shared" si="7"/>
-        <v>CF</v>
-      </c>
-      <c r="G22" s="14" t="str">
-        <f t="shared" si="8"/>
-        <v>1A1</v>
-      </c>
-      <c r="H22" s="18">
-        <f t="shared" si="9"/>
-        <v>1.6666666666666668E-3</v>
-      </c>
-      <c r="I22" s="3"/>
-      <c r="J22" s="3"/>
+        <v>416.66666666666669</v>
+      </c>
       <c r="K22" s="4"/>
       <c r="L22" s="4"/>
     </row>
@@ -1461,23 +1479,29 @@
         <v>16</v>
       </c>
       <c r="E23" s="3">
+        <f t="shared" si="7"/>
+        <v>3.3333333333333335E-3</v>
+      </c>
+      <c r="F23" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>CF</v>
+      </c>
+      <c r="G23" s="14" t="str">
+        <f t="shared" si="9"/>
+        <v>271</v>
+      </c>
+      <c r="H23" s="18">
+        <f t="shared" si="10"/>
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="I23" s="3">
+        <f t="shared" si="11"/>
+        <v>625</v>
+      </c>
+      <c r="J23" s="5">
         <f t="shared" si="6"/>
-        <v>3.3333333333333335E-3</v>
-      </c>
-      <c r="F23" s="11" t="str">
-        <f t="shared" si="7"/>
-        <v>CF</v>
-      </c>
-      <c r="G23" s="14" t="str">
-        <f t="shared" si="8"/>
-        <v>271</v>
-      </c>
-      <c r="H23" s="18">
-        <f t="shared" si="9"/>
-        <v>2.5000000000000001E-3</v>
-      </c>
-      <c r="I23" s="3"/>
-      <c r="J23" s="3"/>
+        <v>625</v>
+      </c>
       <c r="K23" s="4"/>
       <c r="L23" s="4"/>
     </row>
@@ -1495,23 +1519,29 @@
         <v>16</v>
       </c>
       <c r="E24" s="3">
+        <f t="shared" si="7"/>
+        <v>3.3333333333333335E-3</v>
+      </c>
+      <c r="F24" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>CF</v>
+      </c>
+      <c r="G24" s="14" t="str">
+        <f t="shared" si="9"/>
+        <v>318</v>
+      </c>
+      <c r="H24" s="18">
+        <f t="shared" si="10"/>
+        <v>3.1666666666666666E-3</v>
+      </c>
+      <c r="I24" s="3">
+        <f t="shared" si="11"/>
+        <v>792</v>
+      </c>
+      <c r="J24" s="5">
         <f t="shared" si="6"/>
-        <v>3.3333333333333335E-3</v>
-      </c>
-      <c r="F24" s="11" t="str">
-        <f t="shared" si="7"/>
-        <v>CF</v>
-      </c>
-      <c r="G24" s="14" t="str">
-        <f t="shared" si="8"/>
-        <v>318</v>
-      </c>
-      <c r="H24" s="18">
-        <f t="shared" si="9"/>
-        <v>3.1666666666666666E-3</v>
-      </c>
-      <c r="I24" s="3"/>
-      <c r="J24" s="3"/>
+        <v>791.66666666666663</v>
+      </c>
       <c r="K24" s="4"/>
       <c r="L24" s="4"/>
     </row>
@@ -1533,19 +1563,25 @@
         <v>2E-3</v>
       </c>
       <c r="F25" s="12" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>7C</v>
       </c>
       <c r="G25" s="15" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>32</v>
       </c>
       <c r="H25" s="17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>2.0000000000000001E-4</v>
       </c>
-      <c r="I25" s="5"/>
-      <c r="J25" s="5"/>
+      <c r="I25" s="3">
+        <f t="shared" si="11"/>
+        <v>50</v>
+      </c>
+      <c r="J25" s="5">
+        <f t="shared" si="6"/>
+        <v>50.000000000000007</v>
+      </c>
       <c r="K25" s="4"/>
       <c r="L25" s="4"/>
     </row>
@@ -1563,23 +1599,29 @@
         <v>16</v>
       </c>
       <c r="E26" s="5">
-        <f t="shared" ref="E26:E29" si="10">1/A26</f>
+        <f t="shared" ref="E26:E29" si="12">1/A26</f>
         <v>2E-3</v>
       </c>
       <c r="F26" s="12" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>7C</v>
       </c>
       <c r="G26" s="15" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>7D</v>
       </c>
       <c r="H26" s="17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="I26" s="5"/>
-      <c r="J26" s="5"/>
+      <c r="I26" s="3">
+        <f t="shared" si="11"/>
+        <v>125</v>
+      </c>
+      <c r="J26" s="5">
+        <f t="shared" si="6"/>
+        <v>125.00000000000001</v>
+      </c>
       <c r="K26" s="4"/>
       <c r="L26" s="4"/>
     </row>
@@ -1597,23 +1639,29 @@
         <v>16</v>
       </c>
       <c r="E27" s="5">
+        <f t="shared" si="12"/>
+        <v>2E-3</v>
+      </c>
+      <c r="F27" s="12" t="str">
+        <f t="shared" si="8"/>
+        <v>7C</v>
+      </c>
+      <c r="G27" s="15" t="str">
+        <f t="shared" si="9"/>
+        <v>FA</v>
+      </c>
+      <c r="H27" s="17">
         <f t="shared" si="10"/>
-        <v>2E-3</v>
-      </c>
-      <c r="F27" s="12" t="str">
-        <f t="shared" si="7"/>
-        <v>7C</v>
-      </c>
-      <c r="G27" s="15" t="str">
-        <f t="shared" si="8"/>
-        <v>FA</v>
-      </c>
-      <c r="H27" s="17">
-        <f t="shared" si="9"/>
         <v>1E-3</v>
       </c>
-      <c r="I27" s="5"/>
-      <c r="J27" s="5"/>
+      <c r="I27" s="3">
+        <f t="shared" si="11"/>
+        <v>250</v>
+      </c>
+      <c r="J27" s="5">
+        <f t="shared" si="6"/>
+        <v>250.00000000000003</v>
+      </c>
       <c r="K27" s="4"/>
       <c r="L27" s="4"/>
     </row>
@@ -1631,23 +1679,29 @@
         <v>16</v>
       </c>
       <c r="E28" s="5">
+        <f t="shared" si="12"/>
+        <v>2E-3</v>
+      </c>
+      <c r="F28" s="12" t="str">
+        <f t="shared" si="8"/>
+        <v>7C</v>
+      </c>
+      <c r="G28" s="15" t="str">
+        <f t="shared" si="9"/>
+        <v>177</v>
+      </c>
+      <c r="H28" s="17">
         <f t="shared" si="10"/>
-        <v>2E-3</v>
-      </c>
-      <c r="F28" s="12" t="str">
-        <f t="shared" si="7"/>
-        <v>7C</v>
-      </c>
-      <c r="G28" s="15" t="str">
-        <f t="shared" si="8"/>
-        <v>177</v>
-      </c>
-      <c r="H28" s="17">
-        <f t="shared" si="9"/>
         <v>1.5E-3</v>
       </c>
-      <c r="I28" s="5"/>
-      <c r="J28" s="5"/>
+      <c r="I28" s="3">
+        <f t="shared" si="11"/>
+        <v>375</v>
+      </c>
+      <c r="J28" s="5">
+        <f t="shared" si="6"/>
+        <v>375</v>
+      </c>
       <c r="K28" s="4"/>
       <c r="L28" s="4"/>
     </row>
@@ -1665,23 +1719,29 @@
         <v>16</v>
       </c>
       <c r="E29" s="5">
+        <f t="shared" si="12"/>
+        <v>2E-3</v>
+      </c>
+      <c r="F29" s="12" t="str">
+        <f t="shared" si="8"/>
+        <v>7C</v>
+      </c>
+      <c r="G29" s="15" t="str">
+        <f t="shared" si="9"/>
+        <v>1DB</v>
+      </c>
+      <c r="H29" s="17">
         <f t="shared" si="10"/>
-        <v>2E-3</v>
-      </c>
-      <c r="F29" s="12" t="str">
-        <f t="shared" si="7"/>
-        <v>7C</v>
-      </c>
-      <c r="G29" s="15" t="str">
-        <f t="shared" si="8"/>
-        <v>1DB</v>
-      </c>
-      <c r="H29" s="17">
-        <f t="shared" si="9"/>
         <v>1.9E-3</v>
       </c>
-      <c r="I29" s="5"/>
-      <c r="J29" s="5"/>
+      <c r="I29" s="3">
+        <f t="shared" si="11"/>
+        <v>475</v>
+      </c>
+      <c r="J29" s="5">
+        <f>(B29*E29)/((1/C29)*16)</f>
+        <v>475</v>
+      </c>
       <c r="K29" s="4"/>
       <c r="L29" s="4"/>
     </row>
@@ -1703,19 +1763,25 @@
         <v>1E-3</v>
       </c>
       <c r="F30" s="11" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>3E</v>
       </c>
       <c r="G30" s="14" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>19</v>
       </c>
       <c r="H30" s="18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1E-4</v>
       </c>
-      <c r="I30" s="3"/>
-      <c r="J30" s="3"/>
+      <c r="I30" s="3">
+        <f t="shared" si="11"/>
+        <v>25</v>
+      </c>
+      <c r="J30" s="5">
+        <f t="shared" ref="J30:J34" si="13">(B30*E30)/((1/C30)*16)</f>
+        <v>25.000000000000004</v>
+      </c>
       <c r="K30" s="4"/>
       <c r="L30" s="4"/>
     </row>
@@ -1733,23 +1799,29 @@
         <v>16</v>
       </c>
       <c r="E31" s="3">
-        <f t="shared" ref="E31:E34" si="11">1/A31</f>
+        <f t="shared" ref="E31:E34" si="14">1/A31</f>
         <v>1E-3</v>
       </c>
       <c r="F31" s="11" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>3E</v>
       </c>
       <c r="G31" s="14" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>3F</v>
       </c>
       <c r="H31" s="18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>2.5000000000000001E-4</v>
       </c>
-      <c r="I31" s="3"/>
-      <c r="J31" s="3"/>
+      <c r="I31" s="3">
+        <f t="shared" si="11"/>
+        <v>63</v>
+      </c>
+      <c r="J31" s="5">
+        <f t="shared" si="13"/>
+        <v>62.500000000000007</v>
+      </c>
       <c r="K31" s="4"/>
       <c r="L31" s="4"/>
     </row>
@@ -1767,23 +1839,29 @@
         <v>16</v>
       </c>
       <c r="E32" s="3">
+        <f t="shared" si="14"/>
+        <v>1E-3</v>
+      </c>
+      <c r="F32" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>3E</v>
+      </c>
+      <c r="G32" s="14" t="str">
+        <f t="shared" si="9"/>
+        <v>7D</v>
+      </c>
+      <c r="H32" s="18">
+        <f t="shared" si="10"/>
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="I32" s="3">
         <f t="shared" si="11"/>
-        <v>1E-3</v>
-      </c>
-      <c r="F32" s="11" t="str">
-        <f t="shared" si="7"/>
-        <v>3E</v>
-      </c>
-      <c r="G32" s="14" t="str">
-        <f t="shared" si="8"/>
-        <v>7D</v>
-      </c>
-      <c r="H32" s="18">
-        <f t="shared" si="9"/>
-        <v>5.0000000000000001E-4</v>
-      </c>
-      <c r="I32" s="3"/>
-      <c r="J32" s="3"/>
+        <v>125</v>
+      </c>
+      <c r="J32" s="5">
+        <f t="shared" si="13"/>
+        <v>125.00000000000001</v>
+      </c>
       <c r="K32" s="4"/>
       <c r="L32" s="4"/>
     </row>
@@ -1801,23 +1879,29 @@
         <v>16</v>
       </c>
       <c r="E33" s="3">
+        <f t="shared" si="14"/>
+        <v>1E-3</v>
+      </c>
+      <c r="F33" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>3E</v>
+      </c>
+      <c r="G33" s="14" t="str">
+        <f t="shared" si="9"/>
+        <v>BC</v>
+      </c>
+      <c r="H33" s="18">
+        <f t="shared" si="10"/>
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="I33" s="3">
         <f t="shared" si="11"/>
-        <v>1E-3</v>
-      </c>
-      <c r="F33" s="11" t="str">
-        <f t="shared" si="7"/>
-        <v>3E</v>
-      </c>
-      <c r="G33" s="14" t="str">
-        <f t="shared" si="8"/>
-        <v>BC</v>
-      </c>
-      <c r="H33" s="18">
-        <f t="shared" si="9"/>
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="I33" s="3"/>
-      <c r="J33" s="3"/>
+        <v>188</v>
+      </c>
+      <c r="J33" s="5">
+        <f t="shared" si="13"/>
+        <v>187.5</v>
+      </c>
       <c r="K33" s="4"/>
       <c r="L33" s="4"/>
     </row>
@@ -1835,25 +1919,628 @@
         <v>16</v>
       </c>
       <c r="E34" s="3">
+        <f t="shared" si="14"/>
+        <v>1E-3</v>
+      </c>
+      <c r="F34" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>3E</v>
+      </c>
+      <c r="G34" s="14" t="str">
+        <f t="shared" si="9"/>
+        <v>EE</v>
+      </c>
+      <c r="H34" s="18">
+        <f t="shared" si="10"/>
+        <v>9.5E-4</v>
+      </c>
+      <c r="I34" s="3">
         <f t="shared" si="11"/>
-        <v>1E-3</v>
-      </c>
-      <c r="F34" s="11" t="str">
-        <f t="shared" si="7"/>
-        <v>3E</v>
-      </c>
-      <c r="G34" s="14" t="str">
-        <f t="shared" si="8"/>
-        <v>EE</v>
-      </c>
-      <c r="H34" s="18">
-        <f t="shared" si="9"/>
-        <v>9.5E-4</v>
-      </c>
-      <c r="I34" s="3"/>
-      <c r="J34" s="3"/>
+        <v>238</v>
+      </c>
+      <c r="J34" s="5">
+        <f t="shared" si="13"/>
+        <v>237.5</v>
+      </c>
       <c r="K34" s="4"/>
       <c r="L34" s="4"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F36" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="G36" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="H36" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="I36" s="2"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37" s="3">
+        <v>300</v>
+      </c>
+      <c r="B37" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="C37" s="3">
+        <v>4000000</v>
+      </c>
+      <c r="D37" s="3">
+        <v>16</v>
+      </c>
+      <c r="E37" s="3">
+        <f>1/A37</f>
+        <v>3.3333333333333335E-3</v>
+      </c>
+      <c r="F37" s="11" t="str">
+        <f>DEC2HEX(ROUND((E37/(4*(2.5*10^-7)*D37))-1,0))</f>
+        <v>CF</v>
+      </c>
+      <c r="G37" s="14" t="str">
+        <f t="shared" ref="G37:G51" si="15">DEC2HEX((B37*E37)/((1/C37)*16))</f>
+        <v>53</v>
+      </c>
+      <c r="H37" s="18">
+        <f>(B37*E37)</f>
+        <v>3.3333333333333338E-4</v>
+      </c>
+      <c r="I37" s="3">
+        <f>HEX2DEC(G37)</f>
+        <v>83</v>
+      </c>
+      <c r="J37">
+        <f>IF(G20=G37,1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A38" s="3">
+        <v>300</v>
+      </c>
+      <c r="B38" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="C38" s="3">
+        <v>4000000</v>
+      </c>
+      <c r="D38" s="3">
+        <v>16</v>
+      </c>
+      <c r="E38" s="3">
+        <f t="shared" ref="E38:E41" si="16">1/A38</f>
+        <v>3.3333333333333335E-3</v>
+      </c>
+      <c r="F38" s="11" t="str">
+        <f t="shared" ref="F38:F51" si="17">DEC2HEX(ROUND((E38/(4*(2.5*10^-7)*D38))-1,0))</f>
+        <v>CF</v>
+      </c>
+      <c r="G38" s="14" t="str">
+        <f t="shared" si="15"/>
+        <v>D0</v>
+      </c>
+      <c r="H38" s="18">
+        <f t="shared" ref="H38:H51" si="18">(B38*E38)</f>
+        <v>8.3333333333333339E-4</v>
+      </c>
+      <c r="I38" s="3">
+        <f t="shared" ref="I38:I51" si="19">HEX2DEC(G38)</f>
+        <v>208</v>
+      </c>
+      <c r="J38">
+        <f t="shared" ref="J38:J51" si="20">IF(G21=G38,1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A39" s="3">
+        <v>300</v>
+      </c>
+      <c r="B39" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C39" s="3">
+        <v>4000000</v>
+      </c>
+      <c r="D39" s="3">
+        <v>16</v>
+      </c>
+      <c r="E39" s="3">
+        <f t="shared" si="16"/>
+        <v>3.3333333333333335E-3</v>
+      </c>
+      <c r="F39" s="11" t="str">
+        <f t="shared" si="17"/>
+        <v>CF</v>
+      </c>
+      <c r="G39" s="14" t="str">
+        <f t="shared" si="15"/>
+        <v>1A0</v>
+      </c>
+      <c r="H39" s="18">
+        <f t="shared" si="18"/>
+        <v>1.6666666666666668E-3</v>
+      </c>
+      <c r="I39" s="3">
+        <f t="shared" si="19"/>
+        <v>416</v>
+      </c>
+      <c r="J39">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A40" s="3">
+        <v>300</v>
+      </c>
+      <c r="B40" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="C40" s="3">
+        <v>4000000</v>
+      </c>
+      <c r="D40" s="3">
+        <v>16</v>
+      </c>
+      <c r="E40" s="3">
+        <f t="shared" si="16"/>
+        <v>3.3333333333333335E-3</v>
+      </c>
+      <c r="F40" s="11" t="str">
+        <f t="shared" si="17"/>
+        <v>CF</v>
+      </c>
+      <c r="G40" s="14" t="str">
+        <f t="shared" si="15"/>
+        <v>271</v>
+      </c>
+      <c r="H40" s="18">
+        <f t="shared" si="18"/>
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="I40" s="3">
+        <f t="shared" si="19"/>
+        <v>625</v>
+      </c>
+      <c r="J40">
+        <f t="shared" si="20"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A41" s="3">
+        <v>300</v>
+      </c>
+      <c r="B41" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="C41" s="3">
+        <v>4000000</v>
+      </c>
+      <c r="D41" s="3">
+        <v>16</v>
+      </c>
+      <c r="E41" s="3">
+        <f t="shared" si="16"/>
+        <v>3.3333333333333335E-3</v>
+      </c>
+      <c r="F41" s="11" t="str">
+        <f t="shared" si="17"/>
+        <v>CF</v>
+      </c>
+      <c r="G41" s="14" t="str">
+        <f t="shared" si="15"/>
+        <v>317</v>
+      </c>
+      <c r="H41" s="18">
+        <f t="shared" si="18"/>
+        <v>3.1666666666666666E-3</v>
+      </c>
+      <c r="I41" s="3">
+        <f t="shared" si="19"/>
+        <v>791</v>
+      </c>
+      <c r="J41">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>500</v>
+      </c>
+      <c r="B42" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C42" s="5">
+        <v>4000000</v>
+      </c>
+      <c r="D42" s="5">
+        <v>16</v>
+      </c>
+      <c r="E42" s="5">
+        <f>1/A42</f>
+        <v>2E-3</v>
+      </c>
+      <c r="F42" s="12" t="str">
+        <f t="shared" si="17"/>
+        <v>7C</v>
+      </c>
+      <c r="G42" s="15" t="str">
+        <f>DEC2HEX((B42*E42)/((1/C42)*16))</f>
+        <v>32</v>
+      </c>
+      <c r="H42" s="17">
+        <f t="shared" si="18"/>
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="I42" s="3">
+        <f t="shared" si="19"/>
+        <v>50</v>
+      </c>
+      <c r="J42">
+        <f t="shared" si="20"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>500</v>
+      </c>
+      <c r="B43" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C43" s="5">
+        <v>4000000</v>
+      </c>
+      <c r="D43" s="5">
+        <v>16</v>
+      </c>
+      <c r="E43" s="5">
+        <f t="shared" ref="E43:E46" si="21">1/A43</f>
+        <v>2E-3</v>
+      </c>
+      <c r="F43" s="12" t="str">
+        <f t="shared" si="17"/>
+        <v>7C</v>
+      </c>
+      <c r="G43" s="15" t="str">
+        <f t="shared" si="15"/>
+        <v>7D</v>
+      </c>
+      <c r="H43" s="17">
+        <f t="shared" si="18"/>
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="I43" s="3">
+        <f t="shared" si="19"/>
+        <v>125</v>
+      </c>
+      <c r="J43">
+        <f t="shared" si="20"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>500</v>
+      </c>
+      <c r="B44" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C44" s="5">
+        <v>4000000</v>
+      </c>
+      <c r="D44" s="5">
+        <v>16</v>
+      </c>
+      <c r="E44" s="5">
+        <f t="shared" si="21"/>
+        <v>2E-3</v>
+      </c>
+      <c r="F44" s="12" t="str">
+        <f t="shared" si="17"/>
+        <v>7C</v>
+      </c>
+      <c r="G44" s="15" t="str">
+        <f t="shared" si="15"/>
+        <v>FA</v>
+      </c>
+      <c r="H44" s="17">
+        <f t="shared" si="18"/>
+        <v>1E-3</v>
+      </c>
+      <c r="I44" s="3">
+        <f t="shared" si="19"/>
+        <v>250</v>
+      </c>
+      <c r="J44">
+        <f t="shared" si="20"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <v>500</v>
+      </c>
+      <c r="B45" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="C45" s="5">
+        <v>4000000</v>
+      </c>
+      <c r="D45" s="5">
+        <v>16</v>
+      </c>
+      <c r="E45" s="5">
+        <f t="shared" si="21"/>
+        <v>2E-3</v>
+      </c>
+      <c r="F45" s="12" t="str">
+        <f t="shared" si="17"/>
+        <v>7C</v>
+      </c>
+      <c r="G45" s="15" t="str">
+        <f t="shared" si="15"/>
+        <v>177</v>
+      </c>
+      <c r="H45" s="17">
+        <f t="shared" si="18"/>
+        <v>1.5E-3</v>
+      </c>
+      <c r="I45" s="3">
+        <f t="shared" si="19"/>
+        <v>375</v>
+      </c>
+      <c r="J45">
+        <f t="shared" si="20"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>500</v>
+      </c>
+      <c r="B46" s="1">
+        <v>0.95</v>
+      </c>
+      <c r="C46" s="5">
+        <v>4000000</v>
+      </c>
+      <c r="D46" s="5">
+        <v>16</v>
+      </c>
+      <c r="E46" s="5">
+        <f t="shared" si="21"/>
+        <v>2E-3</v>
+      </c>
+      <c r="F46" s="12" t="str">
+        <f t="shared" si="17"/>
+        <v>7C</v>
+      </c>
+      <c r="G46" s="15" t="str">
+        <f t="shared" si="15"/>
+        <v>1DB</v>
+      </c>
+      <c r="H46" s="17">
+        <f t="shared" si="18"/>
+        <v>1.9E-3</v>
+      </c>
+      <c r="I46" s="3">
+        <f t="shared" si="19"/>
+        <v>475</v>
+      </c>
+      <c r="J46">
+        <f t="shared" si="20"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A47" s="3">
+        <v>1000</v>
+      </c>
+      <c r="B47" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="C47" s="3">
+        <v>4000000</v>
+      </c>
+      <c r="D47" s="3">
+        <v>16</v>
+      </c>
+      <c r="E47" s="3">
+        <f>1/A47</f>
+        <v>1E-3</v>
+      </c>
+      <c r="F47" s="11" t="str">
+        <f t="shared" si="17"/>
+        <v>3E</v>
+      </c>
+      <c r="G47" s="14" t="str">
+        <f t="shared" si="15"/>
+        <v>19</v>
+      </c>
+      <c r="H47" s="18">
+        <f t="shared" si="18"/>
+        <v>1E-4</v>
+      </c>
+      <c r="I47" s="3">
+        <f t="shared" si="19"/>
+        <v>25</v>
+      </c>
+      <c r="J47">
+        <f t="shared" si="20"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A48" s="3">
+        <v>1000</v>
+      </c>
+      <c r="B48" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="C48" s="3">
+        <v>4000000</v>
+      </c>
+      <c r="D48" s="3">
+        <v>16</v>
+      </c>
+      <c r="E48" s="3">
+        <f t="shared" ref="E48:E51" si="22">1/A48</f>
+        <v>1E-3</v>
+      </c>
+      <c r="F48" s="11" t="str">
+        <f t="shared" si="17"/>
+        <v>3E</v>
+      </c>
+      <c r="G48" s="14" t="str">
+        <f t="shared" si="15"/>
+        <v>3E</v>
+      </c>
+      <c r="H48" s="18">
+        <f t="shared" si="18"/>
+        <v>2.5000000000000001E-4</v>
+      </c>
+      <c r="I48" s="3">
+        <f t="shared" si="19"/>
+        <v>62</v>
+      </c>
+      <c r="J48">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A49" s="3">
+        <v>1000</v>
+      </c>
+      <c r="B49" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C49" s="3">
+        <v>4000000</v>
+      </c>
+      <c r="D49" s="3">
+        <v>16</v>
+      </c>
+      <c r="E49" s="3">
+        <f t="shared" si="22"/>
+        <v>1E-3</v>
+      </c>
+      <c r="F49" s="11" t="str">
+        <f t="shared" si="17"/>
+        <v>3E</v>
+      </c>
+      <c r="G49" s="14" t="str">
+        <f t="shared" si="15"/>
+        <v>7D</v>
+      </c>
+      <c r="H49" s="18">
+        <f t="shared" si="18"/>
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="I49" s="3">
+        <f t="shared" si="19"/>
+        <v>125</v>
+      </c>
+      <c r="J49">
+        <f t="shared" si="20"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A50" s="3">
+        <v>1000</v>
+      </c>
+      <c r="B50" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="C50" s="3">
+        <v>4000000</v>
+      </c>
+      <c r="D50" s="3">
+        <v>16</v>
+      </c>
+      <c r="E50" s="3">
+        <f t="shared" si="22"/>
+        <v>1E-3</v>
+      </c>
+      <c r="F50" s="11" t="str">
+        <f t="shared" si="17"/>
+        <v>3E</v>
+      </c>
+      <c r="G50" s="14" t="str">
+        <f t="shared" si="15"/>
+        <v>BB</v>
+      </c>
+      <c r="H50" s="18">
+        <f t="shared" si="18"/>
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="I50" s="3">
+        <f t="shared" si="19"/>
+        <v>187</v>
+      </c>
+      <c r="J50">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A51" s="3">
+        <v>1000</v>
+      </c>
+      <c r="B51" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="C51" s="3">
+        <v>4000000</v>
+      </c>
+      <c r="D51" s="3">
+        <v>16</v>
+      </c>
+      <c r="E51" s="3">
+        <f t="shared" si="22"/>
+        <v>1E-3</v>
+      </c>
+      <c r="F51" s="11" t="str">
+        <f t="shared" si="17"/>
+        <v>3E</v>
+      </c>
+      <c r="G51" s="14" t="str">
+        <f t="shared" si="15"/>
+        <v>ED</v>
+      </c>
+      <c r="H51" s="18">
+        <f t="shared" si="18"/>
+        <v>9.5E-4</v>
+      </c>
+      <c r="I51" s="3">
+        <f t="shared" si="19"/>
+        <v>237</v>
+      </c>
+      <c r="J51">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>